<commit_message>
fixes #46. Adds languages and adds Fairy, Owlfolk, Rabbitfolk, and Tortle
</commit_message>
<xml_diff>
--- a/Programming_Tools/Backgrounds (Editable).xlsx
+++ b/Programming_Tools/Backgrounds (Editable).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub Clones\www\wangte\Programming_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C344DD7E-BF85-4AA1-B79E-0F34C802D9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66272B14-B0D6-43C3-BBE8-69FC69802EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="4230" windowWidth="14955" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21210" yWindow="7320" windowWidth="14955" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2275,9 +2275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:K16"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>